<commit_message>
started analyszing the data
</commit_message>
<xml_diff>
--- a/Experiments/Overview_Experiments.xlsx
+++ b/Experiments/Overview_Experiments.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christine Nussbaum\Documents\Arbeit\Forschungsprojekte\2024_Simultaneus_Adaptation\Experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christine Nussbaum\Documents\Arbeit\Forschungsprojekte\2025_Simultaneous_Adaptation\Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E275851-2551-4991-A065-0F1347B52318}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF67D2F-BC9C-4D21-A1D6-21B63716C946}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
   <si>
     <t>Exp1</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>3.4.6</t>
+  </si>
+  <si>
+    <t>March 2025</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -184,7 +190,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="8" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -213,9 +218,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -499,7 +504,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,16 +684,19 @@
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -708,19 +716,25 @@
       <c r="E10" t="s">
         <v>36</v>
       </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
       <c r="C11">
         <v>122</v>
       </c>
       <c r="D11">
         <v>195</v>
       </c>
-      <c r="E11" s="2">
-        <v>74</v>
+      <c r="E11" s="4">
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -736,8 +750,8 @@
       <c r="D12">
         <v>99</v>
       </c>
-      <c r="E12" s="2">
-        <v>37</v>
+      <c r="E12" s="4">
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -753,8 +767,8 @@
       <c r="D13">
         <v>47</v>
       </c>
-      <c r="E13" s="2">
-        <v>27</v>
+      <c r="E13" s="4">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
analysis preparation of all experiments
</commit_message>
<xml_diff>
--- a/Experiments/Overview_Experiments.xlsx
+++ b/Experiments/Overview_Experiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christine Nussbaum\Documents\Arbeit\Forschungsprojekte\2025_Simultaneous_Adaptation\Experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Christine\Arbeit\06_Forschungsprojekte\2025_Simultaneous_Adaptation\Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9AD96A-7A2F-4FFD-91D6-751218E4699D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB610C8-07BF-4FBB-91A1-54AC7CDB802E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview_allExperiments" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
   <si>
     <t>Exp1</t>
   </si>
@@ -187,6 +187,15 @@
   </si>
   <si>
     <t>Hearing Impairments</t>
+  </si>
+  <si>
+    <t>5 -&gt; check</t>
+  </si>
+  <si>
+    <t>1 (my test dataset)</t>
+  </si>
+  <si>
+    <t>4 -&gt; Check</t>
   </si>
 </sst>
 </file>
@@ -533,7 +542,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G18:G19"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +806,7 @@
         <v>47</v>
       </c>
       <c r="E13" s="4">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -807,6 +816,18 @@
       <c r="B15">
         <v>0</v>
       </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -815,36 +836,96 @@
       <c r="B16" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B17">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>36</v>
+      </c>
+      <c r="D17">
+        <v>39</v>
+      </c>
+      <c r="E17">
+        <v>29</v>
+      </c>
+      <c r="F17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B18">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working on analysis of Exp3
</commit_message>
<xml_diff>
--- a/Experiments/Overview_Experiments.xlsx
+++ b/Experiments/Overview_Experiments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Christine\Arbeit\06_Forschungsprojekte\2025_Simultaneous_Adaptation\Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8719C4C-74F1-4ACB-801C-A719CD0C6DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D0FE4B-2790-4C70-AA8B-B05DA24EFA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
   <si>
     <t>Exp1</t>
   </si>
@@ -189,9 +189,6 @@
     <t>Hearing Impairments</t>
   </si>
   <si>
-    <t>5 -&gt; check</t>
-  </si>
-  <si>
     <t>1 (my test dataset)</t>
   </si>
   <si>
@@ -217,6 +214,12 @@
   </si>
   <si>
     <t>2 -&gt; one kept, one removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 removed, 2 kept in </t>
+  </si>
+  <si>
+    <t>3 (wg missings)</t>
   </si>
 </sst>
 </file>
@@ -564,7 +567,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +828,7 @@
         <v>45</v>
       </c>
       <c r="D13">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E13" s="4">
         <v>36</v>
@@ -841,11 +844,11 @@
       <c r="C15">
         <v>2</v>
       </c>
-      <c r="D15">
-        <v>1</v>
+      <c r="D15" t="s">
+        <v>64</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -856,19 +859,19 @@
         <v>48</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>49</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -953,12 +956,12 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24">
         <v>33</v>
@@ -975,7 +978,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25">
         <v>43</v>
@@ -992,7 +995,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" s="6">
         <v>7.0000000000000007E-2</v>
@@ -1009,7 +1012,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>